<commit_message>
remove bypass ratio = 100
</commit_message>
<xml_diff>
--- a/airplane_database_copieVF.xlsx
+++ b/airplane_database_copieVF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Drive\My work\ENAC-intern\Generic-Airplane-Model-GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1E02EC-200F-496F-8C9B-95FD35D98973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225EA08-5825-4717-B322-F06BB195A5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airplane_database_copieVF_test" sheetId="1" r:id="rId1"/>
@@ -2379,7 +2379,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -2860,7 +2860,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -3219,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AG303" sqref="AG303"/>
+    <sheetView tabSelected="1" topLeftCell="I58" workbookViewId="0">
+      <selection activeCell="Y200" sqref="Y187:Y200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10738,9 +10738,6 @@
       <c r="X65" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="Y65" s="1">
-        <v>100</v>
-      </c>
       <c r="Z65" s="1" t="s">
         <v>60</v>
       </c>
@@ -10854,9 +10851,6 @@
       <c r="X66" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="Y66" s="1">
-        <v>100</v>
-      </c>
       <c r="Z66" s="1" t="s">
         <v>60</v>
       </c>
@@ -10970,9 +10964,6 @@
       <c r="X67" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="Y67" s="1">
-        <v>100</v>
-      </c>
       <c r="Z67" s="1" t="s">
         <v>60</v>
       </c>
@@ -11086,9 +11077,6 @@
       <c r="X68" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Y68" s="1">
-        <v>100</v>
-      </c>
       <c r="Z68" s="1" t="s">
         <v>60</v>
       </c>
@@ -11202,9 +11190,6 @@
       <c r="X69" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="Y69" s="1">
-        <v>100</v>
-      </c>
       <c r="Z69" s="1" t="s">
         <v>60</v>
       </c>
@@ -11318,9 +11303,6 @@
       <c r="X70" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="Y70" s="1">
-        <v>100</v>
-      </c>
       <c r="Z70" s="1" t="s">
         <v>60</v>
       </c>
@@ -11434,9 +11416,6 @@
       <c r="X71" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="Y71" s="1">
-        <v>100</v>
-      </c>
       <c r="Z71" s="1" t="s">
         <v>60</v>
       </c>
@@ -11550,9 +11529,6 @@
       <c r="X72" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Y72" s="1">
-        <v>100</v>
-      </c>
       <c r="Z72" s="1" t="s">
         <v>60</v>
       </c>
@@ -11666,9 +11642,6 @@
       <c r="X73" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="Y73" s="1">
-        <v>100</v>
-      </c>
       <c r="Z73" s="1" t="s">
         <v>60</v>
       </c>
@@ -11782,9 +11755,6 @@
       <c r="X74" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Y74" s="1">
-        <v>100</v>
-      </c>
       <c r="Z74" s="1" t="s">
         <v>229</v>
       </c>
@@ -11898,9 +11868,6 @@
       <c r="X75" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="Y75" s="1">
-        <v>100</v>
-      </c>
       <c r="Z75" s="1" t="s">
         <v>60</v>
       </c>
@@ -12014,9 +11981,6 @@
       <c r="X76" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="Y76" s="1">
-        <v>100</v>
-      </c>
       <c r="Z76" s="1" t="s">
         <v>60</v>
       </c>
@@ -12130,9 +12094,6 @@
       <c r="X77" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="Y77" s="1">
-        <v>100</v>
-      </c>
       <c r="Z77" s="1" t="s">
         <v>60</v>
       </c>
@@ -12246,9 +12207,6 @@
       <c r="X78" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="Y78" s="1">
-        <v>100</v>
-      </c>
       <c r="Z78" s="1" t="s">
         <v>60</v>
       </c>
@@ -12362,9 +12320,6 @@
       <c r="X79" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="Y79" s="1">
-        <v>100</v>
-      </c>
       <c r="Z79" s="1" t="s">
         <v>60</v>
       </c>
@@ -12478,9 +12433,6 @@
       <c r="X80" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="Y80" s="1">
-        <v>100</v>
-      </c>
       <c r="Z80" s="1" t="s">
         <v>60</v>
       </c>
@@ -12594,9 +12546,6 @@
       <c r="X81" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="Y81" s="1">
-        <v>100</v>
-      </c>
       <c r="Z81" s="1" t="s">
         <v>60</v>
       </c>
@@ -12710,9 +12659,6 @@
       <c r="X82" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Y82" s="1">
-        <v>100</v>
-      </c>
       <c r="Z82" s="1" t="s">
         <v>60</v>
       </c>
@@ -12826,9 +12772,6 @@
       <c r="X83" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="Y83" s="1">
-        <v>100</v>
-      </c>
       <c r="Z83" s="1" t="s">
         <v>60</v>
       </c>
@@ -12942,9 +12885,6 @@
       <c r="X84" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="Y84" s="1">
-        <v>100</v>
-      </c>
       <c r="Z84" s="1" t="s">
         <v>60</v>
       </c>
@@ -13058,9 +12998,6 @@
       <c r="X85" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Y85" s="1">
-        <v>100</v>
-      </c>
       <c r="Z85" s="1" t="s">
         <v>60</v>
       </c>
@@ -13174,9 +13111,6 @@
       <c r="X86" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="Y86" s="1">
-        <v>100</v>
-      </c>
       <c r="Z86" s="1" t="s">
         <v>60</v>
       </c>
@@ -13290,9 +13224,6 @@
       <c r="X87" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="Y87" s="1">
-        <v>100</v>
-      </c>
       <c r="Z87" s="1" t="s">
         <v>60</v>
       </c>
@@ -13406,9 +13337,6 @@
       <c r="X88" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="Y88" s="1">
-        <v>100</v>
-      </c>
       <c r="Z88" s="1" t="s">
         <v>60</v>
       </c>
@@ -13522,9 +13450,6 @@
       <c r="X89" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="Y89" s="1">
-        <v>100</v>
-      </c>
       <c r="Z89" s="1" t="s">
         <v>60</v>
       </c>
@@ -13638,9 +13563,6 @@
       <c r="X90" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="Y90" s="1">
-        <v>100</v>
-      </c>
       <c r="Z90" s="1" t="s">
         <v>60</v>
       </c>
@@ -13754,9 +13676,6 @@
       <c r="X91" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="Y91" s="1">
-        <v>100</v>
-      </c>
       <c r="Z91" s="1" t="s">
         <v>60</v>
       </c>
@@ -13870,9 +13789,6 @@
       <c r="X92" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="Y92" s="1">
-        <v>100</v>
-      </c>
       <c r="Z92" s="1" t="s">
         <v>60</v>
       </c>
@@ -13986,9 +13902,6 @@
       <c r="X93" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Y93" s="1">
-        <v>100</v>
-      </c>
       <c r="Z93" s="1" t="s">
         <v>60</v>
       </c>
@@ -14102,9 +14015,6 @@
       <c r="X94" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="Y94" s="1">
-        <v>100</v>
-      </c>
       <c r="Z94" s="1" t="s">
         <v>60</v>
       </c>
@@ -14218,9 +14128,6 @@
       <c r="X95" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Y95" s="1">
-        <v>100</v>
-      </c>
       <c r="Z95" s="1" t="s">
         <v>229</v>
       </c>
@@ -14334,9 +14241,6 @@
       <c r="X96" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="Y96" s="1">
-        <v>100</v>
-      </c>
       <c r="Z96" s="1" t="s">
         <v>229</v>
       </c>
@@ -14450,9 +14354,6 @@
       <c r="X97" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="Y97" s="1">
-        <v>100</v>
-      </c>
       <c r="Z97" s="1" t="s">
         <v>229</v>
       </c>
@@ -14566,9 +14467,6 @@
       <c r="X98" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="Y98" s="1">
-        <v>100</v>
-      </c>
       <c r="Z98" s="1" t="s">
         <v>229</v>
       </c>
@@ -14682,9 +14580,6 @@
       <c r="X99" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="Y99" s="1">
-        <v>100</v>
-      </c>
       <c r="Z99" s="1" t="s">
         <v>229</v>
       </c>
@@ -14798,9 +14693,6 @@
       <c r="X100" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="Y100" s="1">
-        <v>100</v>
-      </c>
       <c r="Z100" s="1" t="s">
         <v>229</v>
       </c>
@@ -14914,9 +14806,6 @@
       <c r="X101" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="Y101" s="1">
-        <v>100</v>
-      </c>
       <c r="Z101" s="1" t="s">
         <v>229</v>
       </c>
@@ -15030,9 +14919,6 @@
       <c r="X102" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="Y102" s="1">
-        <v>100</v>
-      </c>
       <c r="Z102" s="1" t="s">
         <v>229</v>
       </c>
@@ -15146,9 +15032,6 @@
       <c r="X103" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="Y103" s="1">
-        <v>100</v>
-      </c>
       <c r="Z103" s="1" t="s">
         <v>229</v>
       </c>
@@ -15262,9 +15145,6 @@
       <c r="X104" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="Y104" s="1">
-        <v>100</v>
-      </c>
       <c r="Z104" s="1" t="s">
         <v>229</v>
       </c>
@@ -15378,9 +15258,6 @@
       <c r="X105" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="Y105" s="1">
-        <v>100</v>
-      </c>
       <c r="Z105" s="1" t="s">
         <v>229</v>
       </c>
@@ -15494,9 +15371,6 @@
       <c r="X106" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="Y106" s="1">
-        <v>100</v>
-      </c>
       <c r="Z106" s="1" t="s">
         <v>60</v>
       </c>
@@ -15610,9 +15484,6 @@
       <c r="X107" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Y107" s="1">
-        <v>100</v>
-      </c>
       <c r="Z107" s="1" t="s">
         <v>60</v>
       </c>
@@ -15726,9 +15597,6 @@
       <c r="X108" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="Y108" s="1">
-        <v>100</v>
-      </c>
       <c r="Z108" s="1" t="s">
         <v>229</v>
       </c>
@@ -15842,9 +15710,6 @@
       <c r="X109" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="Y109" s="1">
-        <v>100</v>
-      </c>
       <c r="Z109" s="1" t="s">
         <v>229</v>
       </c>
@@ -15958,9 +15823,6 @@
       <c r="X110" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="Y110" s="1">
-        <v>100</v>
-      </c>
       <c r="Z110" s="1" t="s">
         <v>229</v>
       </c>
@@ -16074,9 +15936,6 @@
       <c r="X111" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="Y111" s="1">
-        <v>100</v>
-      </c>
       <c r="Z111" s="1" t="s">
         <v>229</v>
       </c>
@@ -16190,9 +16049,6 @@
       <c r="X112" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="Y112" s="1">
-        <v>100</v>
-      </c>
       <c r="Z112" s="1" t="s">
         <v>60</v>
       </c>
@@ -16306,9 +16162,6 @@
       <c r="X113" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="Y113" s="1">
-        <v>100</v>
-      </c>
       <c r="Z113" s="1" t="s">
         <v>229</v>
       </c>
@@ -16422,9 +16275,6 @@
       <c r="X114" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="Y114" s="1">
-        <v>100</v>
-      </c>
       <c r="Z114" s="1" t="s">
         <v>229</v>
       </c>
@@ -16538,9 +16388,6 @@
       <c r="X115" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="Y115" s="1">
-        <v>100</v>
-      </c>
       <c r="Z115" s="1" t="s">
         <v>229</v>
       </c>
@@ -16654,9 +16501,6 @@
       <c r="X116" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="Y116" s="1">
-        <v>100</v>
-      </c>
       <c r="Z116" s="1" t="s">
         <v>60</v>
       </c>
@@ -16770,9 +16614,6 @@
       <c r="X117" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="Y117" s="1">
-        <v>100</v>
-      </c>
       <c r="Z117" s="1" t="s">
         <v>229</v>
       </c>
@@ -16886,9 +16727,6 @@
       <c r="X118" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="Y118" s="1">
-        <v>100</v>
-      </c>
       <c r="Z118" s="1" t="s">
         <v>229</v>
       </c>
@@ -17002,9 +16840,6 @@
       <c r="X119" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="Y119" s="1">
-        <v>100</v>
-      </c>
       <c r="Z119" s="1" t="s">
         <v>229</v>
       </c>
@@ -17118,9 +16953,6 @@
       <c r="X120" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="Y120" s="1">
-        <v>100</v>
-      </c>
       <c r="Z120" s="1" t="s">
         <v>229</v>
       </c>
@@ -17234,9 +17066,6 @@
       <c r="X121" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="Y121" s="1">
-        <v>100</v>
-      </c>
       <c r="Z121" s="1" t="s">
         <v>229</v>
       </c>
@@ -17350,9 +17179,6 @@
       <c r="X122" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="Y122" s="1">
-        <v>100</v>
-      </c>
       <c r="Z122" s="1" t="s">
         <v>229</v>
       </c>
@@ -17466,9 +17292,6 @@
       <c r="X123" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="Y123" s="1">
-        <v>100</v>
-      </c>
       <c r="Z123" s="1" t="s">
         <v>229</v>
       </c>
@@ -17582,9 +17405,6 @@
       <c r="X124" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="Y124" s="1">
-        <v>100</v>
-      </c>
       <c r="Z124" s="1" t="s">
         <v>229</v>
       </c>
@@ -17698,9 +17518,6 @@
       <c r="X125" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Y125" s="1">
-        <v>100</v>
-      </c>
       <c r="Z125" s="1" t="s">
         <v>60</v>
       </c>
@@ -17814,9 +17631,6 @@
       <c r="X126" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="Y126" s="1">
-        <v>100</v>
-      </c>
       <c r="Z126" s="1" t="s">
         <v>229</v>
       </c>
@@ -17930,9 +17744,6 @@
       <c r="X127" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="Y127" s="1">
-        <v>100</v>
-      </c>
       <c r="Z127" s="1" t="s">
         <v>229</v>
       </c>
@@ -18046,9 +17857,6 @@
       <c r="X128" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="Y128" s="1">
-        <v>100</v>
-      </c>
       <c r="Z128" s="1" t="s">
         <v>229</v>
       </c>
@@ -18162,9 +17970,6 @@
       <c r="X129" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="Y129" s="1">
-        <v>100</v>
-      </c>
       <c r="Z129" s="1" t="s">
         <v>229</v>
       </c>
@@ -18278,9 +18083,6 @@
       <c r="X130" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="Y130" s="1">
-        <v>100</v>
-      </c>
       <c r="Z130" s="1" t="s">
         <v>229</v>
       </c>
@@ -18394,9 +18196,6 @@
       <c r="X131" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="Y131" s="1">
-        <v>100</v>
-      </c>
       <c r="Z131" s="1" t="s">
         <v>229</v>
       </c>
@@ -18510,9 +18309,6 @@
       <c r="X132" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="Y132" s="1">
-        <v>100</v>
-      </c>
       <c r="Z132" s="1" t="s">
         <v>229</v>
       </c>
@@ -18626,9 +18422,6 @@
       <c r="X133" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="Y133" s="1">
-        <v>100</v>
-      </c>
       <c r="Z133" s="1" t="s">
         <v>229</v>
       </c>
@@ -18742,9 +18535,6 @@
       <c r="X134" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="Y134" s="1">
-        <v>100</v>
-      </c>
       <c r="Z134" s="1" t="s">
         <v>229</v>
       </c>
@@ -18858,9 +18648,6 @@
       <c r="X135" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="Y135" s="1">
-        <v>100</v>
-      </c>
       <c r="Z135" s="1" t="s">
         <v>229</v>
       </c>
@@ -18974,9 +18761,6 @@
       <c r="X136" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="Y136" s="1">
-        <v>100</v>
-      </c>
       <c r="Z136" s="1" t="s">
         <v>229</v>
       </c>
@@ -19090,9 +18874,6 @@
       <c r="X137" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="Y137" s="1">
-        <v>100</v>
-      </c>
       <c r="Z137" s="1" t="s">
         <v>229</v>
       </c>
@@ -19206,9 +18987,6 @@
       <c r="X138" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="Y138" s="1">
-        <v>100</v>
-      </c>
       <c r="Z138" s="1" t="s">
         <v>229</v>
       </c>
@@ -19322,9 +19100,6 @@
       <c r="X139" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="Y139" s="1">
-        <v>100</v>
-      </c>
       <c r="Z139" s="1" t="s">
         <v>60</v>
       </c>
@@ -19438,9 +19213,6 @@
       <c r="X140" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="Y140" s="1">
-        <v>100</v>
-      </c>
       <c r="Z140" s="1" t="s">
         <v>229</v>
       </c>
@@ -24890,9 +24662,6 @@
       <c r="X187" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="Y187" s="1">
-        <v>100</v>
-      </c>
       <c r="Z187" s="1" t="s">
         <v>60</v>
       </c>
@@ -25006,9 +24775,6 @@
       <c r="X188" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="Y188" s="1">
-        <v>100</v>
-      </c>
       <c r="Z188" s="1" t="s">
         <v>60</v>
       </c>
@@ -25122,9 +24888,6 @@
       <c r="X189" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="Y189" s="1">
-        <v>100</v>
-      </c>
       <c r="Z189" s="1" t="s">
         <v>60</v>
       </c>
@@ -25238,9 +25001,6 @@
       <c r="X190" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="Y190" s="1">
-        <v>100</v>
-      </c>
       <c r="Z190" s="1" t="s">
         <v>60</v>
       </c>
@@ -25354,9 +25114,6 @@
       <c r="X191" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="Y191" s="1">
-        <v>100</v>
-      </c>
       <c r="Z191" s="1" t="s">
         <v>60</v>
       </c>
@@ -25470,9 +25227,6 @@
       <c r="X192" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="Y192" s="1">
-        <v>100</v>
-      </c>
       <c r="Z192" s="1" t="s">
         <v>60</v>
       </c>
@@ -25586,9 +25340,6 @@
       <c r="X193" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="Y193" s="1">
-        <v>100</v>
-      </c>
       <c r="Z193" s="1" t="s">
         <v>60</v>
       </c>
@@ -25702,9 +25453,6 @@
       <c r="X194" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="Y194" s="1">
-        <v>100</v>
-      </c>
       <c r="Z194" s="1" t="s">
         <v>60</v>
       </c>
@@ -25818,9 +25566,6 @@
       <c r="X195" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="Y195" s="1">
-        <v>100</v>
-      </c>
       <c r="Z195" s="1" t="s">
         <v>60</v>
       </c>
@@ -25934,9 +25679,6 @@
       <c r="X196" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="Y196" s="1">
-        <v>100</v>
-      </c>
       <c r="Z196" s="1" t="s">
         <v>60</v>
       </c>
@@ -26050,9 +25792,6 @@
       <c r="X197" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="Y197" s="1">
-        <v>100</v>
-      </c>
       <c r="Z197" s="1" t="s">
         <v>60</v>
       </c>
@@ -26166,9 +25905,6 @@
       <c r="X198" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="Y198" s="1">
-        <v>100</v>
-      </c>
       <c r="Z198" s="1" t="s">
         <v>60</v>
       </c>
@@ -26282,9 +26018,6 @@
       <c r="X199" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="Y199" s="1">
-        <v>100</v>
-      </c>
       <c r="Z199" s="1" t="s">
         <v>60</v>
       </c>
@@ -26398,9 +26131,6 @@
       <c r="X200" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="Y200" s="1">
-        <v>100</v>
-      </c>
       <c r="Z200" s="1" t="s">
         <v>60</v>
       </c>
@@ -27326,9 +27056,6 @@
       <c r="X208" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="Y208" s="1">
-        <v>100</v>
-      </c>
       <c r="Z208" s="1" t="s">
         <v>60</v>
       </c>
@@ -27442,9 +27169,6 @@
       <c r="X209" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="Y209" s="1">
-        <v>100</v>
-      </c>
       <c r="Z209" s="1" t="s">
         <v>60</v>
       </c>
@@ -27558,9 +27282,6 @@
       <c r="X210" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="Y210" s="1">
-        <v>100</v>
-      </c>
       <c r="Z210" s="1" t="s">
         <v>60</v>
       </c>
@@ -27674,9 +27395,6 @@
       <c r="X211" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="Y211" s="1">
-        <v>100</v>
-      </c>
       <c r="Z211" s="1" t="s">
         <v>60</v>
       </c>
@@ -27790,9 +27508,6 @@
       <c r="X212" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="Y212" s="1">
-        <v>100</v>
-      </c>
       <c r="Z212" s="1" t="s">
         <v>60</v>
       </c>
@@ -27906,9 +27621,6 @@
       <c r="X213" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="Y213" s="1">
-        <v>100</v>
-      </c>
       <c r="Z213" s="1" t="s">
         <v>60</v>
       </c>
@@ -28138,9 +27850,6 @@
       <c r="X215" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="Y215" s="1">
-        <v>100</v>
-      </c>
       <c r="Z215" s="1" t="s">
         <v>60</v>
       </c>
@@ -29066,9 +28775,6 @@
       <c r="X223" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="Y223" s="1">
-        <v>100</v>
-      </c>
       <c r="Z223" s="1" t="s">
         <v>60</v>
       </c>
@@ -29182,9 +28888,6 @@
       <c r="X224" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="Y224" s="1">
-        <v>100</v>
-      </c>
       <c r="Z224" s="1" t="s">
         <v>60</v>
       </c>
@@ -29298,9 +29001,6 @@
       <c r="X225" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="Y225" s="1">
-        <v>100</v>
-      </c>
       <c r="Z225" s="1" t="s">
         <v>60</v>
       </c>
@@ -29414,9 +29114,6 @@
       <c r="X226" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="Y226" s="1">
-        <v>100</v>
-      </c>
       <c r="Z226" s="1" t="s">
         <v>60</v>
       </c>
@@ -29530,9 +29227,6 @@
       <c r="X227" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="Y227" s="1">
-        <v>100</v>
-      </c>
       <c r="Z227" s="1" t="s">
         <v>60</v>
       </c>
@@ -29646,9 +29340,6 @@
       <c r="X228" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="Y228" s="1">
-        <v>100</v>
-      </c>
       <c r="Z228" s="1" t="s">
         <v>60</v>
       </c>
@@ -29762,9 +29453,6 @@
       <c r="X229" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="Y229" s="1">
-        <v>100</v>
-      </c>
       <c r="Z229" s="1" t="s">
         <v>60</v>
       </c>
@@ -29878,9 +29566,6 @@
       <c r="X230" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="Y230" s="1">
-        <v>100</v>
-      </c>
       <c r="Z230" s="1" t="s">
         <v>60</v>
       </c>
@@ -29994,9 +29679,6 @@
       <c r="X231" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="Y231" s="1">
-        <v>100</v>
-      </c>
       <c r="Z231" s="1" t="s">
         <v>60</v>
       </c>
@@ -30110,9 +29792,6 @@
       <c r="X232" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="Y232" s="1">
-        <v>100</v>
-      </c>
       <c r="Z232" s="1" t="s">
         <v>60</v>
       </c>
@@ -30226,9 +29905,6 @@
       <c r="X233" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="Y233" s="1">
-        <v>100</v>
-      </c>
       <c r="Z233" s="1" t="s">
         <v>60</v>
       </c>
@@ -30341,9 +30017,6 @@
       </c>
       <c r="X234" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="Y234" s="1">
-        <v>100</v>
       </c>
       <c r="Z234" s="1" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
saving in the middle of debugging stage
</commit_message>
<xml_diff>
--- a/airplane_database_copieVF.xlsx
+++ b/airplane_database_copieVF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Drive\My work\ENAC-intern\Generic-Airplane-Model-GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enacfr-my.sharepoint.com/personal/dajung_kim_enac_fr/Documents/My work/ENAC-intern/Generic-Airplane-Model-GUI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225EA08-5825-4717-B322-F06BB195A5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5225EA08-5825-4717-B322-F06BB195A5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B59A256-A17A-4046-B694-204E6C436BBF}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airplane_database_copieVF_test" sheetId="1" r:id="rId1"/>
@@ -3219,12 +3219,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I58" workbookViewId="0">
-      <selection activeCell="Y200" sqref="Y187:Y200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="6" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="1"/>
     <col min="12" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -4644,7 +4647,7 @@
         <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E13" t="s">
         <v>77</v>
@@ -4760,7 +4763,7 @@
         <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E14" t="s">
         <v>77</v>
@@ -4876,7 +4879,7 @@
         <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
         <v>77</v>
@@ -4992,7 +4995,7 @@
         <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E16" t="s">
         <v>77</v>
@@ -5108,7 +5111,7 @@
         <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
         <v>77</v>
@@ -5224,7 +5227,7 @@
         <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
         <v>77</v>
@@ -5688,7 +5691,7 @@
         <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
@@ -5804,7 +5807,7 @@
         <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E23" t="s">
         <v>77</v>
@@ -5920,7 +5923,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E24" t="s">
         <v>77</v>
@@ -6036,7 +6039,7 @@
         <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
         <v>77</v>
@@ -6152,7 +6155,7 @@
         <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E26" t="s">
         <v>77</v>
@@ -6268,7 +6271,7 @@
         <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E27" t="s">
         <v>77</v>
@@ -8008,7 +8011,7 @@
         <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E42" t="s">
         <v>77</v>
@@ -8124,7 +8127,7 @@
         <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s">
         <v>77</v>
@@ -8240,7 +8243,7 @@
         <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E44" t="s">
         <v>77</v>
@@ -8356,7 +8359,7 @@
         <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E45" t="s">
         <v>77</v>
@@ -8472,7 +8475,7 @@
         <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E46" t="s">
         <v>77</v>
@@ -8588,7 +8591,7 @@
         <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E47" t="s">
         <v>77</v>
@@ -8704,7 +8707,7 @@
         <v>77</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E48" t="s">
         <v>77</v>
@@ -8820,7 +8823,7 @@
         <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E49" t="s">
         <v>77</v>
@@ -8936,7 +8939,7 @@
         <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E50" t="s">
         <v>77</v>
@@ -9052,7 +9055,7 @@
         <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="E51" t="s">
         <v>77</v>
@@ -12823,7 +12826,7 @@
         <v>77</v>
       </c>
       <c r="D84" t="s">
-        <v>77</v>
+        <v>260</v>
       </c>
       <c r="E84" t="s">
         <v>77</v>

</xml_diff>